<commit_message>
connect database and create 5 entitys
</commit_message>
<xml_diff>
--- a/Document/texts/Book1.xlsx
+++ b/Document/texts/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ProgramJava BKAP\E-Project\Document\texts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2E20E4-BA79-41BD-8E85-43B5A1877922}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CDE0CFD-FF72-4756-9CC2-C1F1034EBB17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{888C53C3-A0FA-4FE4-BDC4-86CD6C505A03}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="122">
   <si>
     <t>cở sở dữ liệu Phần mềm quản lý cửa hàng</t>
   </si>
@@ -105,15 +105,9 @@
     <t>ảnh đại diện</t>
   </si>
   <si>
-    <t>powerful</t>
-  </si>
-  <si>
     <t>tinyint</t>
   </si>
   <si>
-    <t>quyền</t>
-  </si>
-  <si>
     <t>date_created</t>
   </si>
   <si>
@@ -375,9 +369,6 @@
     <t/>
   </si>
   <si>
-    <t>permission</t>
-  </si>
-  <si>
     <t>per_action</t>
   </si>
   <si>
@@ -403,6 +394,9 @@
   </si>
   <si>
     <t>not null, unique</t>
+  </si>
+  <si>
+    <t>groupspermissions</t>
   </si>
 </sst>
 </file>
@@ -512,16 +506,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -530,8 +518,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -849,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{450F4389-CE54-486F-902D-4A69CC3A60F4}">
   <dimension ref="A2:U78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,39 +860,39 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
     </row>
     <row r="3" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="G3" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="H3" s="10"/>
+      <c r="B3" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="G3" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" s="14"/>
     </row>
     <row r="5" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -975,7 +969,7 @@
         <v>13</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -992,16 +986,16 @@
         <v>19</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -1018,16 +1012,16 @@
         <v>20</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -1044,102 +1038,94 @@
         <v>23</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="H10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="F11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="G11" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H13" s="10"/>
+      <c r="G13" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="14"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>1</v>
@@ -1169,10 +1155,10 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="C17" s="11"/>
+      <c r="B17" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C17" s="10"/>
       <c r="F17" s="1" t="s">
         <v>11</v>
       </c>
@@ -1183,21 +1169,21 @@
         <v>13</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F18" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1214,16 +1200,16 @@
         <v>5</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>13</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1234,16 +1220,16 @@
         <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>22</v>
@@ -1261,19 +1247,19 @@
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1285,7 +1271,7 @@
         <v>15</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>13</v>
@@ -1296,68 +1282,68 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="C23" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>22</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G25" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="H25" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1366,27 +1352,27 @@
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="F26" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="C28" s="12"/>
-      <c r="G28" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="H28" s="11"/>
+      <c r="B28" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="15"/>
+      <c r="G28" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
@@ -1451,7 +1437,7 @@
         <v>13</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>11</v>
@@ -1463,7 +1449,7 @@
         <v>13</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1472,10 +1458,10 @@
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="F32" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>22</v>
@@ -1486,87 +1472,87 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F33" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G33" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="H33" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="F34" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>12</v>
@@ -1575,19 +1561,19 @@
         <v>22</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G37" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="H37" s="11"/>
+        <v>51</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="H37" s="10"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>22</v>
@@ -1610,16 +1596,16 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>6</v>
@@ -1636,19 +1622,19 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>7</v>
@@ -1657,24 +1643,24 @@
         <v>13</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>7</v>
@@ -1683,24 +1669,24 @@
         <v>22</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>7</v>
@@ -1709,96 +1695,96 @@
         <v>22</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="C44" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F44" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G44" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G44" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="H44" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B48" s="11" t="s">
+      <c r="B48" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C48" s="10"/>
+      <c r="G48" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="C48" s="11"/>
-      <c r="G48" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="H48" s="11"/>
+      <c r="H48" s="10"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
@@ -1840,16 +1826,16 @@
         <v>10</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H50" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -1863,10 +1849,10 @@
         <v>13</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>7</v>
@@ -1875,24 +1861,24 @@
         <v>8</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G52" s="3" t="s">
         <v>7</v>
@@ -1901,47 +1887,47 @@
         <v>13</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="C53" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F53" s="6"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B56" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="C56" s="14"/>
-      <c r="G56" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="H56" s="11"/>
+      <c r="B56" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C56" s="12"/>
+      <c r="G56" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H56" s="10"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
@@ -1971,16 +1957,16 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>6</v>
@@ -1997,80 +1983,80 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="C60" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H60" s="3" t="s">
         <v>22</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H61" s="3" t="s">
         <v>22</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -2079,16 +2065,16 @@
       <c r="C62" s="6"/>
       <c r="D62" s="6"/>
       <c r="F62" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I62" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -2097,36 +2083,36 @@
       <c r="C63" s="6"/>
       <c r="D63" s="6"/>
       <c r="F63" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G63" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G63" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="H63" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="7"/>
-      <c r="B64" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="C64" s="15"/>
+      <c r="B64" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C64" s="9"/>
       <c r="D64" s="7"/>
       <c r="F64" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -2145,66 +2131,66 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="C68" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="7"/>
-      <c r="B72" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="C72" s="15"/>
+      <c r="B72" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C72" s="9"/>
       <c r="D72" s="7"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2232,7 +2218,7 @@
         <v>8</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2240,59 +2226,66 @@
         <v>11</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B77" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="C77" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A2:U2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G28:H28"/>
     <mergeCell ref="B64:C64"/>
     <mergeCell ref="B72:C72"/>
     <mergeCell ref="G56:H56"/>
@@ -2300,13 +2293,6 @@
     <mergeCell ref="G37:H37"/>
     <mergeCell ref="B48:C48"/>
     <mergeCell ref="G48:H48"/>
-    <mergeCell ref="A2:U2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G28:H28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>